<commit_message>
actualiza graficos - regex
</commit_message>
<xml_diff>
--- a/docs/datos.xlsx
+++ b/docs/datos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucho\Documents\concu defin\TrabajoFinalConcurrente\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDB70AB2-5079-408D-A422-AE6A0E60810C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05736E40-7A6A-4418-B0F5-52E08DB1D6E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{75DF82C1-206C-4805-9326-2C870CF471F6}"/>
   </bookViews>
@@ -301,34 +301,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10.63</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.4</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.4</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.62</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.05</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.6</c:v>
+                  <c:v>12.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.4</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.7</c:v>
+                  <c:v>17.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.8</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.8</c:v>
+                  <c:v>21.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -341,7 +341,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -840,34 +839,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.08</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.2</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.4</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.7</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.2</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.6</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.9</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.03</c:v>
+                  <c:v>18.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.7</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.07</c:v>
+                  <c:v>20.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1383,34 +1382,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.6</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.6</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.7</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.600000000000001</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.4</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.3</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.09</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.7</c:v>
+                  <c:v>20.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.68</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1922,34 +1921,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.6</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.3</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>14.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.600000000000001</c:v>
+                  <c:v>15.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.6</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.74</c:v>
+                  <c:v>20.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.574999999999999</c:v>
+                  <c:v>24.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2448,34 +2447,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>10.63</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.4</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.4</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.62</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.05</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11.6</c:v>
+                  <c:v>12.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.4</c:v>
+                  <c:v>15.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.7</c:v>
+                  <c:v>17.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.8</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.8</c:v>
+                  <c:v>21.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2574,34 +2573,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.08</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.2</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.4</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.7</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.2</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.6</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.9</c:v>
+                  <c:v>15.3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>16.03</c:v>
+                  <c:v>18.2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>16.7</c:v>
+                  <c:v>18.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.07</c:v>
+                  <c:v>20.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2700,34 +2699,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.6</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.6</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.7</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.600000000000001</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.4</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.3</c:v>
+                  <c:v>16.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.09</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26.7</c:v>
+                  <c:v>20.2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>30.68</c:v>
+                  <c:v>21.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2826,34 +2825,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>11.1</c:v>
+                  <c:v>4.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.6</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.3</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20</c:v>
+                  <c:v>14.45</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.600000000000001</c:v>
+                  <c:v>15.1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22.6</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.74</c:v>
+                  <c:v>20.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>26</c:v>
+                  <c:v>20.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.574999999999999</c:v>
+                  <c:v>24.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6272,8 +6271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27D3181E-F4AE-4CFD-A020-D8B5A39D9858}">
   <dimension ref="C3:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O57" sqref="O57"/>
+    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6309,25 +6308,25 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>10.63</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
       <c r="G4">
-        <v>11.08</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I4">
         <v>10</v>
       </c>
       <c r="J4">
-        <v>11.6</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N4">
         <v>10</v>
       </c>
       <c r="O4">
-        <v>11.1</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="5" spans="3:15" x14ac:dyDescent="0.35">
@@ -6335,25 +6334,25 @@
         <v>20</v>
       </c>
       <c r="D5">
-        <v>10.4</v>
+        <v>6.2</v>
       </c>
       <c r="F5">
         <v>20</v>
       </c>
       <c r="G5">
-        <v>11.2</v>
+        <v>6.1</v>
       </c>
       <c r="I5">
         <v>20</v>
       </c>
       <c r="J5">
-        <v>13.6</v>
+        <v>6.1</v>
       </c>
       <c r="N5">
         <v>20</v>
       </c>
       <c r="O5">
-        <v>13.8</v>
+        <v>8.9</v>
       </c>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.35">
@@ -6361,25 +6360,25 @@
         <v>30</v>
       </c>
       <c r="D6">
-        <v>10.4</v>
+        <v>6.6</v>
       </c>
       <c r="F6">
         <v>30</v>
       </c>
       <c r="G6">
-        <v>11.4</v>
+        <v>6.5</v>
       </c>
       <c r="I6">
         <v>30</v>
       </c>
       <c r="J6">
-        <v>14.7</v>
+        <v>6.8</v>
       </c>
       <c r="N6">
         <v>30</v>
       </c>
       <c r="O6">
-        <v>13.6</v>
+        <v>8.8000000000000007</v>
       </c>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.35">
@@ -6387,25 +6386,25 @@
         <v>40</v>
       </c>
       <c r="D7">
-        <v>10.62</v>
+        <v>9.4</v>
       </c>
       <c r="F7">
         <v>40</v>
       </c>
       <c r="G7">
-        <v>13.7</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="I7">
         <v>40</v>
       </c>
       <c r="J7">
-        <v>17.600000000000001</v>
+        <v>9.6</v>
       </c>
       <c r="N7">
         <v>40</v>
       </c>
       <c r="O7" s="1">
-        <v>16.3</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.35">
@@ -6413,25 +6412,25 @@
         <v>50</v>
       </c>
       <c r="D8">
-        <v>11.05</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>50</v>
       </c>
       <c r="G8">
-        <v>11.2</v>
+        <v>12.1</v>
       </c>
       <c r="I8">
         <v>50</v>
       </c>
       <c r="J8">
-        <v>20.6</v>
+        <v>12</v>
       </c>
       <c r="N8">
         <v>50</v>
       </c>
-      <c r="O8" s="1">
-        <v>20</v>
+      <c r="O8">
+        <v>14.45</v>
       </c>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.35">
@@ -6439,25 +6438,25 @@
         <v>60</v>
       </c>
       <c r="D9">
-        <v>11.6</v>
+        <v>12.4</v>
       </c>
       <c r="F9">
         <v>60</v>
       </c>
       <c r="G9">
-        <v>14.6</v>
+        <v>12.7</v>
       </c>
       <c r="I9">
         <v>60</v>
       </c>
       <c r="J9">
-        <v>21.4</v>
+        <v>13.9</v>
       </c>
       <c r="N9">
         <v>60</v>
       </c>
-      <c r="O9" s="1">
-        <v>19.600000000000001</v>
+      <c r="O9">
+        <v>15.1</v>
       </c>
     </row>
     <row r="10" spans="3:15" x14ac:dyDescent="0.35">
@@ -6465,25 +6464,25 @@
         <v>70</v>
       </c>
       <c r="D10">
-        <v>12.4</v>
+        <v>15.2</v>
       </c>
       <c r="F10">
         <v>70</v>
       </c>
       <c r="G10">
-        <v>15.9</v>
+        <v>15.3</v>
       </c>
       <c r="I10">
         <v>70</v>
       </c>
       <c r="J10">
-        <v>24.3</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="N10">
         <v>70</v>
       </c>
-      <c r="O10" s="1">
-        <v>22.6</v>
+      <c r="O10">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="3:15" x14ac:dyDescent="0.35">
@@ -6491,25 +6490,25 @@
         <v>80</v>
       </c>
       <c r="D11">
-        <v>12.7</v>
+        <v>17.8</v>
       </c>
       <c r="F11">
         <v>80</v>
       </c>
       <c r="G11">
-        <v>16.03</v>
+        <v>18.2</v>
       </c>
       <c r="I11">
         <v>80</v>
       </c>
       <c r="J11">
-        <v>27.09</v>
+        <v>17.5</v>
       </c>
       <c r="N11">
         <v>80</v>
       </c>
-      <c r="O11" s="1">
-        <v>25.74</v>
+      <c r="O11">
+        <v>20.3</v>
       </c>
     </row>
     <row r="12" spans="3:15" x14ac:dyDescent="0.35">
@@ -6517,25 +6516,25 @@
         <v>90</v>
       </c>
       <c r="D12">
-        <v>13.8</v>
+        <v>18.5</v>
       </c>
       <c r="F12">
         <v>90</v>
       </c>
       <c r="G12">
-        <v>16.7</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I12">
         <v>90</v>
       </c>
       <c r="J12">
-        <v>26.7</v>
+        <v>20.2</v>
       </c>
       <c r="N12">
         <v>90</v>
       </c>
-      <c r="O12" s="1">
-        <v>26</v>
+      <c r="O12">
+        <v>20.9</v>
       </c>
     </row>
     <row r="13" spans="3:15" x14ac:dyDescent="0.35">
@@ -6543,25 +6542,25 @@
         <v>100</v>
       </c>
       <c r="D13">
-        <v>14.8</v>
+        <v>21.1</v>
       </c>
       <c r="F13">
         <v>100</v>
       </c>
       <c r="G13">
-        <v>16.07</v>
+        <v>20.6</v>
       </c>
       <c r="I13">
         <v>100</v>
       </c>
       <c r="J13">
-        <v>30.68</v>
+        <v>21.9</v>
       </c>
       <c r="N13">
         <v>100</v>
       </c>
-      <c r="O13" s="1">
-        <v>27.574999999999999</v>
+      <c r="O13">
+        <v>24.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>